<commit_message>
Adding ESIIL and CyVerse
</commit_message>
<xml_diff>
--- a/data_map.xlsx
+++ b/data_map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topoa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\posdocs_sinbiose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E53BD1-FD78-45D6-AA5E-47389695C394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084F68A-59EF-4787-93DB-FFCE9241A298}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{852DF55B-3C19-487B-B217-E7483E03ECF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -277,6 +277,24 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>CyVerse</t>
+  </si>
+  <si>
+    <t>Tucson</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>ESIIL</t>
+  </si>
+  <si>
+    <t>Boulder</t>
+  </si>
+  <si>
+    <t>Environmental Data Science Innovation &amp; Inclusion Lab</t>
   </si>
 </sst>
 </file>
@@ -629,14 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D677691C-2D69-40C2-A1E2-BAE1AE193394}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
@@ -1106,6 +1125,64 @@
         <v>68</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17">
+        <v>32.253943</v>
+      </c>
+      <c r="H17">
+        <v>-110.974114</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18">
+        <v>40.022557999999997</v>
+      </c>
+      <c r="H18">
+        <v>-105.250169</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating data and map
</commit_message>
<xml_diff>
--- a/data_map.xlsx
+++ b/data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\posdocs_sinbiose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BEA389-C61E-485D-9899-6FF6B4D85E56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AAAD1-CFD3-42BE-A020-CBCF0B76CB4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{852DF55B-3C19-487B-B217-E7483E03ECF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>ZA</t>
+  </si>
+  <si>
+    <t>BIOTA SYNTHESIS</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
   </si>
 </sst>
 </file>
@@ -662,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D677691C-2D69-40C2-A1E2-BAE1AE193394}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,6 +1233,35 @@
         <v>68</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20">
+        <v>-23.561140000000002</v>
+      </c>
+      <c r="H20">
+        <v>-46.722847000000002</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
active centers, updated map
</commit_message>
<xml_diff>
--- a/data_map.xlsx
+++ b/data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\posdocs_sinbiose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D33DB3-B4EB-4907-993E-E9AA1EA0423B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E319A9-0C7A-4FA8-99D4-7A2DE3D416D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{852DF55B-3C19-487B-B217-E7483E03ECF2}"/>
   </bookViews>
@@ -279,15 +279,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>CyVerse</t>
-  </si>
-  <si>
-    <t>Tucson</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
     <t>African Synthesis Center</t>
   </si>
   <si>
@@ -307,6 +298,15 @@
   </si>
   <si>
     <t>São Paulo</t>
+  </si>
+  <si>
+    <t>ESIIL</t>
+  </si>
+  <si>
+    <t>Boulder</t>
+  </si>
+  <si>
+    <t>Environmental Data Science Innovation &amp; Inclusion Lab</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,16 +1139,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>28</v>
@@ -1157,10 +1157,10 @@
         <v>76</v>
       </c>
       <c r="G17">
-        <v>32.253943</v>
+        <v>40.014986</v>
       </c>
       <c r="H17">
-        <v>-110.974114</v>
+        <v>-105.270546</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>67</v>
@@ -1168,22 +1168,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G18">
         <v>-33.960158</v>
@@ -1197,16 +1197,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
updates in the data and map
</commit_message>
<xml_diff>
--- a/data_map.xlsx
+++ b/data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\posdocs_sinbiose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E319A9-0C7A-4FA8-99D4-7A2DE3D416D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BB3E5B-A30B-4A97-81A0-334432E177D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{852DF55B-3C19-487B-B217-E7483E03ECF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -307,6 +307,45 @@
   </si>
   <si>
     <t>Environmental Data Science Innovation &amp; Inclusion Lab</t>
+  </si>
+  <si>
+    <t>IPBES</t>
+  </si>
+  <si>
+    <t>Bonn</t>
+  </si>
+  <si>
+    <t>Intergovernmental Science-Policy Platform on Biodiversity and Ecosystem Services</t>
+  </si>
+  <si>
+    <t>Science for Nature and People Partnership</t>
+  </si>
+  <si>
+    <t>SNAPP</t>
+  </si>
+  <si>
+    <t>Arlington</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>EU Knowledge and Learning Mechanism on Biodiversity and Ecosystem Services</t>
+  </si>
+  <si>
+    <t>EKLIPSE</t>
+  </si>
+  <si>
+    <t>Lenfest Ocean Programme at The Pew Charitable Trusts</t>
+  </si>
+  <si>
+    <t>Lenfest</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
   </si>
 </sst>
 </file>
@@ -659,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D677691C-2D69-40C2-A1E2-BAE1AE193394}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,6 +1263,122 @@
         <v>67</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20">
+        <v>50.71848</v>
+      </c>
+      <c r="H20">
+        <v>7.1254629999999999</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21">
+        <v>38.877848</v>
+      </c>
+      <c r="H21">
+        <v>-77.089731999999998</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22">
+        <v>51.351638000000001</v>
+      </c>
+      <c r="H22">
+        <v>12.430899999999999</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23">
+        <v>38.897542999999999</v>
+      </c>
+      <c r="H23">
+        <v>-77.026568999999995</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update in data and readme
</commit_message>
<xml_diff>
--- a/data_map.xlsx
+++ b/data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\posdocs_sinbiose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BB3E5B-A30B-4A97-81A0-334432E177D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B2F56B-A8AC-4038-BE58-8A978E0E263F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{852DF55B-3C19-487B-B217-E7483E03ECF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -346,6 +346,27 @@
   </si>
   <si>
     <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Commission of Inquiry on Peatlands</t>
+  </si>
+  <si>
+    <t>IUCN UK Peatland Programme</t>
+  </si>
+  <si>
+    <t>Edinburgh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The UK National Ecosystem Assessment </t>
+  </si>
+  <si>
+    <t>UK NEA</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>General coordinate</t>
   </si>
 </sst>
 </file>
@@ -698,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D677691C-2D69-40C2-A1E2-BAE1AE193394}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +733,7 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,8 +761,11 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -769,8 +793,9 @@
       <c r="I2" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -799,7 +824,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -828,7 +853,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -857,7 +882,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -886,7 +911,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -915,7 +940,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -944,7 +969,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -973,7 +998,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1002,7 +1027,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1031,7 +1056,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -1060,7 +1085,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -1089,7 +1114,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1118,7 +1143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -1147,7 +1172,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1176,7 +1201,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>93</v>
       </c>
@@ -1205,7 +1230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -1234,7 +1259,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1263,7 +1288,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -1292,7 +1317,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1321,7 +1346,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1350,7 +1375,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1378,6 +1403,70 @@
       <c r="I23" s="1" t="s">
         <v>67</v>
       </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24">
+        <v>55.947634999999998</v>
+      </c>
+      <c r="H24">
+        <v>-3.1859769999999998</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25">
+        <v>55.266739999999999</v>
+      </c>
+      <c r="H25">
+        <v>-3.358428</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>